<commit_message>
Added Loadings Plot input form
</commit_message>
<xml_diff>
--- a/PCA_Addin/Examples/AIM084_Thermo_Plasma_results2_example.xlsx
+++ b/PCA_Addin/Examples/AIM084_Thermo_Plasma_results2_example.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="24915" windowHeight="14625" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
-    <sheet name="Chart1" sheetId="6" r:id="rId1"/>
+    <sheet name="Scores Plot" sheetId="6" r:id="rId1"/>
     <sheet name="V Results" sheetId="5" r:id="rId2"/>
     <sheet name="S2 Results" sheetId="4" r:id="rId3"/>
     <sheet name="Quan Table" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -613,8 +613,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -663,17 +663,34 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -747,6 +764,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -815,6 +833,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -883,6 +902,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -960,6 +980,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
@@ -1028,6 +1049,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
@@ -1084,6 +1106,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="6"/>
@@ -1152,37 +1175,52 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="219337472"/>
-        <c:axId val="219339008"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="150566784"/>
+        <c:axId val="150568320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="219337472"/>
+        <c:axId val="150566784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
           <c:min val="-1"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="219339008"/>
+        <c:crossAx val="150568320"/>
         <c:crossesAt val="-1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="219339008"/>
+        <c:axId val="150568320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
           <c:min val="-1"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="219337472"/>
+        <c:crossAx val="150566784"/>
         <c:crossesAt val="-1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1190,20 +1228,35 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1434,32 +1487,47 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="37343232"/>
-        <c:axId val="37340672"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="149978496"/>
+        <c:axId val="149984384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="37343232"/>
+        <c:axId val="149978496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="37340672"/>
+        <c:crossAx val="149984384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="37340672"/>
+        <c:axId val="149984384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="37343232"/>
+        <c:crossAx val="149978496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1467,8 +1535,11 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1482,7 +1553,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="120" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="47" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1493,7 +1564,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8636000" cy="6278562"/>
+    <xdr:ext cx="8673830" cy="6302713"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -1626,6 +1697,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1660,6 +1732,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1835,19 +1908,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>155</v>
       </c>
@@ -1954,7 +2027,7 @@
         <v>-1.0706912931587261E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:35">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>155</v>
       </c>
@@ -2061,7 +2134,7 @@
         <v>-4.1502606008947604E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:35">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>155</v>
       </c>
@@ -2168,7 +2241,7 @@
         <v>-6.7004708520921649E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:35">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>155</v>
       </c>
@@ -2275,7 +2348,7 @@
         <v>-1.0982521375555951E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>155</v>
       </c>
@@ -2382,7 +2455,7 @@
         <v>1.8130756183967322E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>155</v>
       </c>
@@ -2489,7 +2562,7 @@
         <v>-4.8954319035959266E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>158</v>
       </c>
@@ -2596,7 +2669,7 @@
         <v>-0.13930962699474198</v>
       </c>
     </row>
-    <row r="8" spans="1:35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>158</v>
       </c>
@@ -2703,7 +2776,7 @@
         <v>0.3601699343760616</v>
       </c>
     </row>
-    <row r="9" spans="1:35">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>158</v>
       </c>
@@ -2810,7 +2883,7 @@
         <v>0.26738895942499674</v>
       </c>
     </row>
-    <row r="10" spans="1:35">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>158</v>
       </c>
@@ -2917,7 +2990,7 @@
         <v>-1.6570481170617712E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:35">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>158</v>
       </c>
@@ -3024,7 +3097,7 @@
         <v>-0.50242071239295971</v>
       </c>
     </row>
-    <row r="12" spans="1:35">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>160</v>
       </c>
@@ -3131,7 +3204,7 @@
         <v>-0.47135490124883928</v>
       </c>
     </row>
-    <row r="13" spans="1:35">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>160</v>
       </c>
@@ -3238,7 +3311,7 @@
         <v>0.12886307671225333</v>
       </c>
     </row>
-    <row r="14" spans="1:35">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>160</v>
       </c>
@@ -3345,7 +3418,7 @@
         <v>0.22673914494211447</v>
       </c>
     </row>
-    <row r="15" spans="1:35">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>160</v>
       </c>
@@ -3452,7 +3525,7 @@
         <v>-9.3518483723949219E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:35">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>160</v>
       </c>
@@ -3559,7 +3632,7 @@
         <v>-0.18260443423153283</v>
       </c>
     </row>
-    <row r="17" spans="1:35">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>162</v>
       </c>
@@ -3666,7 +3739,7 @@
         <v>-9.1933920229885974E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:35">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>162</v>
       </c>
@@ -3773,7 +3846,7 @@
         <v>-5.544878780924449E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:35">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>162</v>
       </c>
@@ -3880,7 +3953,7 @@
         <v>-2.8654823375105699E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:35">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>162</v>
       </c>
@@ -3987,7 +4060,7 @@
         <v>5.8137348592235821E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:35">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>162</v>
       </c>
@@ -4094,7 +4167,7 @@
         <v>-0.37879343520605385</v>
       </c>
     </row>
-    <row r="22" spans="1:35">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>164</v>
       </c>
@@ -4201,7 +4274,7 @@
         <v>-0.12567748428238745</v>
       </c>
     </row>
-    <row r="23" spans="1:35">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>164</v>
       </c>
@@ -4308,7 +4381,7 @@
         <v>1.0254698283432269E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:35">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>164</v>
       </c>
@@ -4415,7 +4488,7 @@
         <v>3.2052755712054385E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:35">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>164</v>
       </c>
@@ -4522,7 +4595,7 @@
         <v>-2.3947972696559849E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:35">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>164</v>
       </c>
@@ -4629,7 +4702,7 @@
         <v>3.299981476994078E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:35">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>166</v>
       </c>
@@ -4736,7 +4809,7 @@
         <v>-2.8296932550181779E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:35">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>166</v>
       </c>
@@ -4843,7 +4916,7 @@
         <v>-3.2134671026043324E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:35">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>166</v>
       </c>
@@ -4950,7 +5023,7 @@
         <v>4.6402686502862021E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:35">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>168</v>
       </c>
@@ -5057,7 +5130,7 @@
         <v>5.9664763883308672E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:35">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>168</v>
       </c>
@@ -5164,7 +5237,7 @@
         <v>2.5629937885177347E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:35">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>168</v>
       </c>
@@ -5271,7 +5344,7 @@
         <v>6.4543964085999475E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:35">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>168</v>
       </c>
@@ -5378,7 +5451,7 @@
         <v>-1.4462954842948834E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:35">
+    <row r="34" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>168</v>
       </c>
@@ -5491,26 +5564,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -5526,7 +5599,7 @@
         <v>0.19201725952479187</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -5542,7 +5615,7 @@
         <v>0.29594868328994844</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -5558,7 +5631,7 @@
         <v>0.37645508782144466</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -5574,7 +5647,7 @@
         <v>0.4378957288468015</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -5590,7 +5663,7 @@
         <v>0.49534432210320917</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -5606,7 +5679,7 @@
         <v>0.54458516612044261</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
@@ -5622,7 +5695,7 @@
         <v>0.58928869053182642</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
@@ -5638,7 +5711,7 @@
         <v>0.62882627066263308</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9</v>
       </c>
@@ -5654,7 +5727,7 @@
         <v>0.6659702624700653</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>10</v>
       </c>
@@ -5670,7 +5743,7 @@
         <v>0.7026930306888125</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>11</v>
       </c>
@@ -5686,7 +5759,7 @@
         <v>0.73420250149720101</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>12</v>
       </c>
@@ -5702,7 +5775,7 @@
         <v>0.76342582844044804</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>13</v>
       </c>
@@ -5718,7 +5791,7 @@
         <v>0.79110220660327024</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>14</v>
       </c>
@@ -5734,7 +5807,7 @@
         <v>0.8151983195417053</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>15</v>
       </c>
@@ -5750,7 +5823,7 @@
         <v>0.83766371170141685</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>16</v>
       </c>
@@ -5766,7 +5839,7 @@
         <v>0.85693107325625228</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>17</v>
       </c>
@@ -5782,7 +5855,7 @@
         <v>0.87554855496170003</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>18</v>
       </c>
@@ -5798,7 +5871,7 @@
         <v>0.89248245657267411</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>19</v>
       </c>
@@ -5814,7 +5887,7 @@
         <v>0.90791063129605953</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>20</v>
       </c>
@@ -5830,7 +5903,7 @@
         <v>0.92272676302294654</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>21</v>
       </c>
@@ -5846,7 +5919,7 @@
         <v>0.9356210520880438</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>22</v>
       </c>
@@ -5862,7 +5935,7 @@
         <v>0.94568119230692849</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>23</v>
       </c>
@@ -5878,7 +5951,7 @@
         <v>0.9549862449981682</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>24</v>
       </c>
@@ -5894,7 +5967,7 @@
         <v>0.96398281779245487</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>25</v>
       </c>
@@ -5910,7 +5983,7 @@
         <v>0.97147912775344936</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>26</v>
       </c>
@@ -5926,7 +5999,7 @@
         <v>0.97714285671595358</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>27</v>
       </c>
@@ -5942,7 +6015,7 @@
         <v>0.98257570771721325</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>28</v>
       </c>
@@ -5958,7 +6031,7 @@
         <v>0.98754412758435473</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>29</v>
       </c>
@@ -5974,7 +6047,7 @@
         <v>0.99186293313933116</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>30</v>
       </c>
@@ -5990,7 +6063,7 @@
         <v>0.99496759080870334</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>31</v>
       </c>
@@ -6006,7 +6079,7 @@
         <v>0.99769686810134384</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>32</v>
       </c>
@@ -6022,7 +6095,7 @@
         <v>0.99912725051871321</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>33</v>
       </c>
@@ -6038,7 +6111,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>34</v>
       </c>
@@ -6050,7 +6123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B39">
         <f>SUM(B5:B38)</f>
         <v>1928.5437183843401</v>
@@ -6063,20 +6136,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EX35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:154">
+    <row r="1" spans="1:154" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6540,7 +6613,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="2" spans="1:154">
+    <row r="2" spans="1:154" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>154</v>
       </c>
@@ -7004,7 +7077,7 @@
         <v>82072.345653569006</v>
       </c>
     </row>
-    <row r="3" spans="1:154">
+    <row r="3" spans="1:154" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>156</v>
       </c>
@@ -7468,7 +7541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:154">
+    <row r="4" spans="1:154" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>169</v>
       </c>
@@ -7932,7 +8005,7 @@
         <v>78213.312568942303</v>
       </c>
     </row>
-    <row r="5" spans="1:154">
+    <row r="5" spans="1:154" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>175</v>
       </c>
@@ -8396,7 +8469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:154">
+    <row r="6" spans="1:154" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>182</v>
       </c>
@@ -8860,7 +8933,7 @@
         <v>40578.664610731801</v>
       </c>
     </row>
-    <row r="7" spans="1:154">
+    <row r="7" spans="1:154" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>188</v>
       </c>
@@ -9324,7 +9397,7 @@
         <v>61635.447946004002</v>
       </c>
     </row>
-    <row r="8" spans="1:154">
+    <row r="8" spans="1:154" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>157</v>
       </c>
@@ -9788,7 +9861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:154">
+    <row r="9" spans="1:154" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>170</v>
       </c>
@@ -10252,7 +10325,7 @@
         <v>86395.295374598005</v>
       </c>
     </row>
-    <row r="10" spans="1:154">
+    <row r="10" spans="1:154" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>176</v>
       </c>
@@ -10716,7 +10789,7 @@
         <v>51122.217962774899</v>
       </c>
     </row>
-    <row r="11" spans="1:154">
+    <row r="11" spans="1:154" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>183</v>
       </c>
@@ -11180,7 +11253,7 @@
         <v>40517.0084326793</v>
       </c>
     </row>
-    <row r="12" spans="1:154">
+    <row r="12" spans="1:154" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>189</v>
       </c>
@@ -11644,7 +11717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:154">
+    <row r="13" spans="1:154" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>159</v>
       </c>
@@ -12108,7 +12181,7 @@
         <v>49685.029422781001</v>
       </c>
     </row>
-    <row r="14" spans="1:154">
+    <row r="14" spans="1:154" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>171</v>
       </c>
@@ -12572,7 +12645,7 @@
         <v>82724.503685555901</v>
       </c>
     </row>
-    <row r="15" spans="1:154">
+    <row r="15" spans="1:154" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>177</v>
       </c>
@@ -13036,7 +13109,7 @@
         <v>52492.6116613185</v>
       </c>
     </row>
-    <row r="16" spans="1:154">
+    <row r="16" spans="1:154" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>184</v>
       </c>
@@ -13500,7 +13573,7 @@
         <v>46030.568765491902</v>
       </c>
     </row>
-    <row r="17" spans="1:154">
+    <row r="17" spans="1:154" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>190</v>
       </c>
@@ -13964,7 +14037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:154">
+    <row r="18" spans="1:154" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>161</v>
       </c>
@@ -14428,7 +14501,7 @@
         <v>59334.800789756096</v>
       </c>
     </row>
-    <row r="19" spans="1:154">
+    <row r="19" spans="1:154" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>172</v>
       </c>
@@ -14892,7 +14965,7 @@
         <v>97781.902714064505</v>
       </c>
     </row>
-    <row r="20" spans="1:154">
+    <row r="20" spans="1:154" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>178</v>
       </c>
@@ -15356,7 +15429,7 @@
         <v>31879.751732115299</v>
       </c>
     </row>
-    <row r="21" spans="1:154">
+    <row r="21" spans="1:154" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>185</v>
       </c>
@@ -15820,7 +15893,7 @@
         <v>39469.501930929502</v>
       </c>
     </row>
-    <row r="22" spans="1:154">
+    <row r="22" spans="1:154" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>191</v>
       </c>
@@ -16284,7 +16357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:154">
+    <row r="23" spans="1:154" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>163</v>
       </c>
@@ -16748,7 +16821,7 @@
         <v>95035.331899025507</v>
       </c>
     </row>
-    <row r="24" spans="1:154">
+    <row r="24" spans="1:154" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>173</v>
       </c>
@@ -17212,7 +17285,7 @@
         <v>55139.134820752399</v>
       </c>
     </row>
-    <row r="25" spans="1:154">
+    <row r="25" spans="1:154" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>179</v>
       </c>
@@ -17676,7 +17749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:154">
+    <row r="26" spans="1:154" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>186</v>
       </c>
@@ -18140,7 +18213,7 @@
         <v>14068.310927482</v>
       </c>
     </row>
-    <row r="27" spans="1:154">
+    <row r="27" spans="1:154" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>192</v>
       </c>
@@ -18604,7 +18677,7 @@
         <v>36368.9093502088</v>
       </c>
     </row>
-    <row r="28" spans="1:154">
+    <row r="28" spans="1:154" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>165</v>
       </c>
@@ -19068,7 +19141,7 @@
         <v>129945.31324310999</v>
       </c>
     </row>
-    <row r="29" spans="1:154">
+    <row r="29" spans="1:154" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>180</v>
       </c>
@@ -19532,7 +19605,7 @@
         <v>47.906045532226599</v>
       </c>
     </row>
-    <row r="30" spans="1:154">
+    <row r="30" spans="1:154" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>193</v>
       </c>
@@ -19996,7 +20069,7 @@
         <v>64464.379782283497</v>
       </c>
     </row>
-    <row r="31" spans="1:154">
+    <row r="31" spans="1:154" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>167</v>
       </c>
@@ -20460,7 +20533,7 @@
         <v>82824.826798599606</v>
       </c>
     </row>
-    <row r="32" spans="1:154">
+    <row r="32" spans="1:154" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>174</v>
       </c>
@@ -20924,7 +20997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:154">
+    <row r="33" spans="1:154" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>181</v>
       </c>
@@ -21388,7 +21461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:154">
+    <row r="34" spans="1:154" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>187</v>
       </c>
@@ -21852,7 +21925,7 @@
         <v>35343.256565858501</v>
       </c>
     </row>
-    <row r="35" spans="1:154">
+    <row r="35" spans="1:154" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>194</v>
       </c>

</xml_diff>